<commit_message>
fixed up patient, drug, and physician edit tests not having dynamic waits
</commit_message>
<xml_diff>
--- a/QA/QATests.xlsx
+++ b/QA/QATests.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sadik\Desktop\College\System\Capston\QA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sadik\Desktop\School\College\Capston\Project\QA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53AD7A09-50CA-4736-B08F-4D0F6368D500}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57E1D85C-EC97-45D1-9379-514FA51C0807}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -503,7 +503,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
added user signup test, password reset test, and also modified the delete test to delete user created in signup test and also add dynamic waits on edit tests
</commit_message>
<xml_diff>
--- a/QA/QATests.xlsx
+++ b/QA/QATests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sadik\Desktop\School\College\Capston\Project\QA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57E1D85C-EC97-45D1-9379-514FA51C0807}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C854FC03-0BDA-408C-A99E-FC1A96EF01E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="30">
   <si>
     <t>RESULT</t>
   </si>
@@ -36,15 +36,6 @@
     <t>PASS</t>
   </si>
   <si>
-    <t>US1</t>
-  </si>
-  <si>
-    <t>US2</t>
-  </si>
-  <si>
-    <t>US5</t>
-  </si>
-  <si>
     <t>US6</t>
   </si>
   <si>
@@ -112,6 +103,18 @@
   </si>
   <si>
     <t>TEST CASE</t>
+  </si>
+  <si>
+    <t>US2DeleteUser</t>
+  </si>
+  <si>
+    <t>US1SignUp</t>
+  </si>
+  <si>
+    <t>US3PasswordReset</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Email confirmation portion is not tested as we have no test email to automate it with</t>
   </si>
 </sst>
 </file>
@@ -504,7 +507,7 @@
   <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -516,7 +519,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -527,17 +530,26 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>27</v>
+      </c>
+      <c r="B2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>26</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C4" t="s">
         <v>2</v>
@@ -545,7 +557,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C5" t="s">
         <v>2</v>
@@ -553,52 +565,58 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>28</v>
+      </c>
+      <c r="B6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C15" t="s">
         <v>2</v>
@@ -606,12 +624,12 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C17" t="s">
         <v>2</v>
@@ -619,12 +637,12 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C19" t="s">
         <v>2</v>
@@ -632,12 +650,12 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C21" t="s">
         <v>2</v>
@@ -645,12 +663,12 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C23" t="s">
         <v>2</v>
@@ -658,12 +676,12 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C25" t="s">
         <v>2</v>
@@ -671,7 +689,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modified some files to work better for qa testing
</commit_message>
<xml_diff>
--- a/QA/QATests.xlsx
+++ b/QA/QATests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sadik\Desktop\School\College\Capston\Project\QA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C854FC03-0BDA-408C-A99E-FC1A96EF01E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00C684F9-9D41-40E6-B8D6-714F75ADDCCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="30">
   <si>
     <t>RESULT</t>
   </si>
@@ -36,9 +36,6 @@
     <t>PASS</t>
   </si>
   <si>
-    <t>US6</t>
-  </si>
-  <si>
     <t>US7</t>
   </si>
   <si>
@@ -115,6 +112,9 @@
   </si>
   <si>
     <t xml:space="preserve"> Email confirmation portion is not tested as we have no test email to automate it with</t>
+  </si>
+  <si>
+    <t>US4CreateOrder</t>
   </si>
 </sst>
 </file>
@@ -507,7 +507,7 @@
   <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -519,7 +519,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -530,10 +530,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
@@ -541,7 +541,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C3" t="s">
         <v>2</v>
@@ -549,7 +549,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C4" t="s">
         <v>2</v>
@@ -557,7 +557,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C5" t="s">
         <v>2</v>
@@ -565,10 +565,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" t="s">
         <v>28</v>
-      </c>
-      <c r="B6" t="s">
-        <v>29</v>
       </c>
       <c r="C6" t="s">
         <v>2</v>
@@ -576,47 +576,50 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>3</v>
+        <v>29</v>
+      </c>
+      <c r="C7" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C15" t="s">
         <v>2</v>
@@ -624,12 +627,12 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C17" t="s">
         <v>2</v>
@@ -637,12 +640,12 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C19" t="s">
         <v>2</v>
@@ -650,12 +653,12 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C21" t="s">
         <v>2</v>
@@ -663,12 +666,12 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C23" t="s">
         <v>2</v>
@@ -676,12 +679,12 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C25" t="s">
         <v>2</v>
@@ -689,7 +692,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added Create Order tests, Reject Order tests, Amend Order Tests, Verify Order Tests, as well as added a MultiWait utility class that allows us to use dynamic waits easier for in the future
</commit_message>
<xml_diff>
--- a/QA/QATests.xlsx
+++ b/QA/QATests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sadik\Desktop\School\College\Capston\Project\QA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00C684F9-9D41-40E6-B8D6-714F75ADDCCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34070E9C-0224-4367-AD89-9B0982AD18EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -507,7 +507,7 @@
   <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
US11TimeOut Added Updated the QA excel sheet
</commit_message>
<xml_diff>
--- a/QA/QATests.xlsx
+++ b/QA/QATests.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sadik\Desktop\School\College\Capston\Project\QA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\CAPSTONE\Pharmacy-Tech-Capston\QA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34070E9C-0224-4367-AD89-9B0982AD18EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEE3EE53-5A60-4220-A378-E39A159C47E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9705" yWindow="2070" windowWidth="17835" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="32">
   <si>
     <t>RESULT</t>
   </si>
@@ -36,21 +36,12 @@
     <t>PASS</t>
   </si>
   <si>
-    <t>US7</t>
-  </si>
-  <si>
-    <t>US8</t>
-  </si>
-  <si>
     <t>US9</t>
   </si>
   <si>
     <t>US10</t>
   </si>
   <si>
-    <t>US11</t>
-  </si>
-  <si>
     <t>US12</t>
   </si>
   <si>
@@ -115,6 +106,21 @@
   </si>
   <si>
     <t>US4CreateOrder</t>
+  </si>
+  <si>
+    <t>US7RejectOrder</t>
+  </si>
+  <si>
+    <t>US8AmendOrder</t>
+  </si>
+  <si>
+    <t>US7VerifyOrder</t>
+  </si>
+  <si>
+    <t>Testing this can be done. Commented out because of long wait time.</t>
+  </si>
+  <si>
+    <t>US11TimeOut</t>
   </si>
 </sst>
 </file>
@@ -504,10 +510,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -519,7 +525,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -530,10 +536,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
@@ -541,7 +547,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C3" t="s">
         <v>2</v>
@@ -549,7 +555,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s">
         <v>2</v>
@@ -557,7 +563,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C5" t="s">
         <v>2</v>
@@ -565,10 +571,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B6" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C6" t="s">
         <v>2</v>
@@ -576,7 +582,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C7" t="s">
         <v>2</v>
@@ -584,120 +590,131 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>3</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>4</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>8</v>
+        <v>31</v>
+      </c>
+      <c r="B13" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>18</v>
-      </c>
-      <c r="C15" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>10</v>
+        <v>15</v>
+      </c>
+      <c r="C16" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>19</v>
-      </c>
-      <c r="C17" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>11</v>
+        <v>16</v>
+      </c>
+      <c r="C18" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>20</v>
-      </c>
-      <c r="C19" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>12</v>
+        <v>17</v>
+      </c>
+      <c r="C20" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>21</v>
-      </c>
-      <c r="C21" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>13</v>
+        <v>18</v>
+      </c>
+      <c r="C22" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>22</v>
-      </c>
-      <c r="C23" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>14</v>
+        <v>19</v>
+      </c>
+      <c r="C24" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>23</v>
-      </c>
-      <c r="C25" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>15</v>
+        <v>20</v>
+      </c>
+      <c r="C26" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="C2:C627">
+  <conditionalFormatting sqref="C2:C628">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"FAIL"</formula>
     </cfRule>

</xml_diff>

<commit_message>
updated old code. Added view orders page US17. Excel updated
</commit_message>
<xml_diff>
--- a/QA/QATests.xlsx
+++ b/QA/QATests.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sadik\Desktop\School\College\Capston\Project\QA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\CAPSTONE\Pharmacy-Tech-Capston\QA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4A25B9B-2E97-474B-9870-40761ADDCC3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E482031-C8F3-4645-BF2E-67EE3F6C8B0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10815" yWindow="1350" windowWidth="17835" windowHeight="12630" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="33">
   <si>
     <t>RESULT</t>
   </si>
@@ -51,9 +51,6 @@
     <t>US15</t>
   </si>
   <si>
-    <t>US17</t>
-  </si>
-  <si>
     <t>US19</t>
   </si>
   <si>
@@ -124,6 +121,9 @@
   </si>
   <si>
     <t>US5UploadImage</t>
+  </si>
+  <si>
+    <t>US17ViewOrders</t>
   </si>
 </sst>
 </file>
@@ -515,8 +515,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -528,7 +528,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -539,10 +539,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
@@ -550,7 +550,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C3" t="s">
         <v>2</v>
@@ -558,7 +558,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s">
         <v>2</v>
@@ -566,7 +566,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C5" t="s">
         <v>2</v>
@@ -574,10 +574,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" t="s">
         <v>24</v>
-      </c>
-      <c r="B6" t="s">
-        <v>25</v>
       </c>
       <c r="C6" t="s">
         <v>2</v>
@@ -585,7 +585,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C7" t="s">
         <v>2</v>
@@ -593,7 +593,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C8" t="s">
         <v>2</v>
@@ -601,7 +601,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C9" t="s">
         <v>2</v>
@@ -609,7 +609,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C10" t="s">
         <v>2</v>
@@ -617,7 +617,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C11" t="s">
         <v>2</v>
@@ -635,10 +635,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C14" t="s">
         <v>2</v>
@@ -656,7 +656,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C17" t="s">
         <v>2</v>
@@ -669,7 +669,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C19" t="s">
         <v>2</v>
@@ -677,12 +677,15 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>8</v>
+        <v>32</v>
+      </c>
+      <c r="C20" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C21" t="s">
         <v>2</v>
@@ -690,12 +693,12 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C23" t="s">
         <v>2</v>
@@ -703,12 +706,12 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C25" t="s">
         <v>2</v>
@@ -716,12 +719,12 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C27" t="s">
         <v>2</v>
@@ -729,7 +732,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added print order test
</commit_message>
<xml_diff>
--- a/QA/QATests.xlsx
+++ b/QA/QATests.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\CAPSTONE\Pharmacy-Tech-Capston\QA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sadik\Desktop\School\College\Capston\Project\QA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E482031-C8F3-4645-BF2E-67EE3F6C8B0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC92F0FD-07D9-45D7-8586-3F46E355B77F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10815" yWindow="1350" windowWidth="17835" windowHeight="12630" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33510" yWindow="2070" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -42,9 +42,6 @@
     <t>US10</t>
   </si>
   <si>
-    <t>US12</t>
-  </si>
-  <si>
     <t>US13</t>
   </si>
   <si>
@@ -123,7 +120,10 @@
     <t>US5UploadImage</t>
   </si>
   <si>
-    <t>US17ViewOrders</t>
+    <t>US12ViewOrders</t>
+  </si>
+  <si>
+    <t>US17</t>
   </si>
 </sst>
 </file>
@@ -515,7 +515,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
@@ -528,7 +528,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -539,10 +539,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
@@ -550,7 +550,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C3" t="s">
         <v>2</v>
@@ -558,7 +558,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
         <v>2</v>
@@ -566,7 +566,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C5" t="s">
         <v>2</v>
@@ -574,10 +574,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" t="s">
         <v>23</v>
-      </c>
-      <c r="B6" t="s">
-        <v>24</v>
       </c>
       <c r="C6" t="s">
         <v>2</v>
@@ -585,7 +585,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C7" t="s">
         <v>2</v>
@@ -593,7 +593,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C8" t="s">
         <v>2</v>
@@ -601,7 +601,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C9" t="s">
         <v>2</v>
@@ -609,7 +609,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C10" t="s">
         <v>2</v>
@@ -617,7 +617,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C11" t="s">
         <v>2</v>
@@ -635,10 +635,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C14" t="s">
         <v>2</v>
@@ -646,17 +646,20 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>5</v>
+        <v>31</v>
+      </c>
+      <c r="C15" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C17" t="s">
         <v>2</v>
@@ -664,12 +667,12 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C19" t="s">
         <v>2</v>
@@ -679,13 +682,10 @@
       <c r="A20" t="s">
         <v>32</v>
       </c>
-      <c r="C20" t="s">
-        <v>2</v>
-      </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C21" t="s">
         <v>2</v>
@@ -693,12 +693,12 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C23" t="s">
         <v>2</v>
@@ -706,12 +706,12 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C25" t="s">
         <v>2</v>
@@ -719,12 +719,12 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C27" t="s">
         <v>2</v>
@@ -732,7 +732,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
small commit to merge
</commit_message>
<xml_diff>
--- a/QA/QATests.xlsx
+++ b/QA/QATests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sadik\Desktop\College\System\Capston\QA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53AD7A09-50CA-4736-B08F-4D0F6368D500}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83D12388-910A-48D3-BCF3-D3A8AF525AFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -503,7 +503,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
added QA Tests for Printing and Reprinting orders
</commit_message>
<xml_diff>
--- a/QA/QATests.xlsx
+++ b/QA/QATests.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sadik\Desktop\School\College\Capston\Project\QA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sadik\Desktop\College\System\Capston\QA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC92F0FD-07D9-45D7-8586-3F46E355B77F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{225BE6E2-9520-4195-9641-874344EF00CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33510" yWindow="2070" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="35">
   <si>
     <t>RESULT</t>
   </si>
@@ -36,12 +36,6 @@
     <t>PASS</t>
   </si>
   <si>
-    <t>US9</t>
-  </si>
-  <si>
-    <t>US10</t>
-  </si>
-  <si>
     <t>US13</t>
   </si>
   <si>
@@ -124,6 +118,18 @@
   </si>
   <si>
     <t>US17</t>
+  </si>
+  <si>
+    <t>US9PrintOrderToPDF</t>
+  </si>
+  <si>
+    <t>US9PrintOrderToPrinter</t>
+  </si>
+  <si>
+    <t>US10RePrintOrderToPDF</t>
+  </si>
+  <si>
+    <t>US10RePrintOrderToPrinter</t>
   </si>
 </sst>
 </file>
@@ -513,22 +519,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C28"/>
+  <dimension ref="A1:C30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.85546875" customWidth="1"/>
+    <col min="1" max="1" width="26.85546875" customWidth="1"/>
     <col min="2" max="2" width="90" customWidth="1"/>
     <col min="3" max="3" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -539,10 +545,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s">
         <v>21</v>
-      </c>
-      <c r="B2" t="s">
-        <v>23</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
@@ -550,7 +556,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C3" t="s">
         <v>2</v>
@@ -558,7 +564,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
         <v>2</v>
@@ -566,7 +572,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
         <v>2</v>
@@ -574,10 +580,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C6" t="s">
         <v>2</v>
@@ -585,7 +591,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C7" t="s">
         <v>2</v>
@@ -593,7 +599,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C8" t="s">
         <v>2</v>
@@ -601,7 +607,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C9" t="s">
         <v>2</v>
@@ -609,7 +615,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C10" t="s">
         <v>2</v>
@@ -617,7 +623,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C11" t="s">
         <v>2</v>
@@ -625,20 +631,23 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>3</v>
+        <v>31</v>
+      </c>
+      <c r="C12" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>4</v>
+        <v>32</v>
+      </c>
+      <c r="C13" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>29</v>
-      </c>
-      <c r="B14" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="C14" t="s">
         <v>2</v>
@@ -646,7 +655,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C15" t="s">
         <v>2</v>
@@ -654,12 +663,18 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>5</v>
+        <v>27</v>
+      </c>
+      <c r="B16" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="C17" t="s">
         <v>2</v>
@@ -667,12 +682,12 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C19" t="s">
         <v>2</v>
@@ -680,12 +695,12 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>32</v>
+        <v>4</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C21" t="s">
         <v>2</v>
@@ -693,12 +708,12 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>7</v>
+        <v>30</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C23" t="s">
         <v>2</v>
@@ -706,12 +721,12 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C25" t="s">
         <v>2</v>
@@ -719,12 +734,12 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C27" t="s">
         <v>2</v>
@@ -732,12 +747,25 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>10</v>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>16</v>
+      </c>
+      <c r="C29" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="C2:C629">
+  <conditionalFormatting sqref="C2:C631">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"FAIL"</formula>
     </cfRule>

</xml_diff>

<commit_message>
Added User story tests for adding and deleting Drugs, Physicians, and Patients. Also, modified edit drug, physician, and patient to only edit test drugs, physicians or patients.
</commit_message>
<xml_diff>
--- a/QA/QATests.xlsx
+++ b/QA/QATests.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sadik\Desktop\College\System\Capston\QA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sadik\Desktop\School\College\Capston\Project\QA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{225BE6E2-9520-4195-9641-874344EF00CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32792A17-7F1D-4545-BD58-885B714BE54D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="39">
   <si>
     <t>RESULT</t>
   </si>
@@ -36,24 +36,6 @@
     <t>PASS</t>
   </si>
   <si>
-    <t>US13</t>
-  </si>
-  <si>
-    <t>US15</t>
-  </si>
-  <si>
-    <t>US19</t>
-  </si>
-  <si>
-    <t>US21</t>
-  </si>
-  <si>
-    <t>US23</t>
-  </si>
-  <si>
-    <t>US25</t>
-  </si>
-  <si>
     <t>US3ValidLogin</t>
   </si>
   <si>
@@ -105,9 +87,6 @@
     <t>US7VerifyOrder</t>
   </si>
   <si>
-    <t>Testing this can be done. Commented out because of long wait time.</t>
-  </si>
-  <si>
     <t>US11TimeOut</t>
   </si>
   <si>
@@ -117,9 +96,6 @@
     <t>US12ViewOrders</t>
   </si>
   <si>
-    <t>US17</t>
-  </si>
-  <si>
     <t>US9PrintOrderToPDF</t>
   </si>
   <si>
@@ -130,6 +106,42 @@
   </si>
   <si>
     <t>US10RePrintOrderToPrinter</t>
+  </si>
+  <si>
+    <t>US13AddDrugSingle</t>
+  </si>
+  <si>
+    <t>US13AddDrugBulk</t>
+  </si>
+  <si>
+    <t>US15DeleteDrugSingle</t>
+  </si>
+  <si>
+    <t>US15DeleteDrugMulti</t>
+  </si>
+  <si>
+    <t>US17AddPhysicianSingle</t>
+  </si>
+  <si>
+    <t>US17AddPhysicianBulk</t>
+  </si>
+  <si>
+    <t>US19DeletePhysicianSingle</t>
+  </si>
+  <si>
+    <t>US19DeletePhysicianMulti</t>
+  </si>
+  <si>
+    <t>US21AddPatientSingle</t>
+  </si>
+  <si>
+    <t>US21AddPatientBulk</t>
+  </si>
+  <si>
+    <t>US23DeletePatientSingle</t>
+  </si>
+  <si>
+    <t>US23DeletePatientMulti</t>
   </si>
 </sst>
 </file>
@@ -519,10 +531,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C30"/>
+  <dimension ref="A1:C35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -534,7 +546,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -545,10 +557,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
@@ -556,7 +568,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
         <v>2</v>
@@ -564,7 +576,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C4" t="s">
         <v>2</v>
@@ -572,7 +584,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C5" t="s">
         <v>2</v>
@@ -580,10 +592,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C6" t="s">
         <v>2</v>
@@ -591,7 +603,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C7" t="s">
         <v>2</v>
@@ -599,7 +611,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="C8" t="s">
         <v>2</v>
@@ -607,7 +619,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C9" t="s">
         <v>2</v>
@@ -615,7 +627,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C10" t="s">
         <v>2</v>
@@ -623,7 +635,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C11" t="s">
         <v>2</v>
@@ -631,7 +643,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="C12" t="s">
         <v>2</v>
@@ -639,7 +651,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="C13" t="s">
         <v>2</v>
@@ -647,7 +659,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="C14" t="s">
         <v>2</v>
@@ -655,7 +667,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="C15" t="s">
         <v>2</v>
@@ -663,10 +675,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>27</v>
-      </c>
-      <c r="B16" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C16" t="s">
         <v>2</v>
@@ -674,7 +683,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="C17" t="s">
         <v>2</v>
@@ -682,12 +691,15 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>3</v>
+        <v>27</v>
+      </c>
+      <c r="C18" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="C19" t="s">
         <v>2</v>
@@ -695,12 +707,15 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="C20" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="C21" t="s">
         <v>2</v>
@@ -710,10 +725,13 @@
       <c r="A22" t="s">
         <v>30</v>
       </c>
+      <c r="C22" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C23" t="s">
         <v>2</v>
@@ -721,12 +739,15 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>5</v>
+        <v>31</v>
+      </c>
+      <c r="C24" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="C25" t="s">
         <v>2</v>
@@ -734,12 +755,15 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>6</v>
+        <v>7</v>
+      </c>
+      <c r="C26" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="C27" t="s">
         <v>2</v>
@@ -747,12 +771,15 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>7</v>
+        <v>34</v>
+      </c>
+      <c r="C28" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C29" t="s">
         <v>2</v>
@@ -760,12 +787,55 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>8</v>
+        <v>35</v>
+      </c>
+      <c r="C30" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>36</v>
+      </c>
+      <c r="C31" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>9</v>
+      </c>
+      <c r="C32" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>37</v>
+      </c>
+      <c r="C33" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>38</v>
+      </c>
+      <c r="C34" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>10</v>
+      </c>
+      <c r="C35" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="C2:C631">
+  <conditionalFormatting sqref="C2:C637">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"FAIL"</formula>
     </cfRule>

</xml_diff>